<commit_message>
rename var and file
</commit_message>
<xml_diff>
--- a/variable/pe_course_of_disease_parameters.xlsx
+++ b/variable/pe_course_of_disease_parameters.xlsx
@@ -1027,7 +1027,7 @@
         <v>1.584685705803562</v>
       </c>
       <c r="N8" t="n">
-        <v>1.400419826865503</v>
+        <v>1.394972424910905</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
         <v>6.92146915001084</v>
       </c>
       <c r="N9" t="n">
-        <v>5.154612012878062</v>
+        <v>5.195268805464966</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1175,7 +1175,7 @@
         <v>0.9999999999999999</v>
       </c>
       <c r="N10" t="n">
-        <v>0.9712209319348002</v>
+        <v>0.9718373744617498</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1471,7 +1471,7 @@
         <v>1.939016773699552</v>
       </c>
       <c r="N14" t="n">
-        <v>0.8450817305550029</v>
+        <v>0.8228798080182611</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1545,7 +1545,7 @@
         <v>8.977582782619464</v>
       </c>
       <c r="N15" t="n">
-        <v>6.328888642894489</v>
+        <v>6.521367423249766</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1619,7 +1619,7 @@
         <v>-3.055577329282006e-28</v>
       </c>
       <c r="N16" t="n">
-        <v>-3.12223149998713e-25</v>
+        <v>-2.858093891259109e-25</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>2.418210880366879</v>
       </c>
       <c r="N25" t="n">
-        <v>0.9076704466754872</v>
+        <v>0.900329279790903</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2359,7 +2359,7 @@
         <v>14.43087199443731</v>
       </c>
       <c r="N26" t="n">
-        <v>10.09574315209524</v>
+        <v>10.21081454111628</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>

</xml_diff>